<commit_message>
Instructions NJR to Excel and completed for <55 Female
</commit_message>
<xml_diff>
--- a/data/55-64_Female_first_revision.xlsx
+++ b/data/55-64_Female_first_revision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/KNIPS/code/KNIPS-Semi-Markov/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{717B2BA7-4759-4B27-B8E0-7C8C40283AFD}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB6B13B1-8800-45EC-8B41-9ED86E8D1DB5}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rcs_first_revision_mean" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="37">
   <si>
     <t>bound1</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>dxb:_d_rcs3</t>
+  </si>
+  <si>
+    <t>_d_rcs3</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:E16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -496,16 +499,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-5.6911350000000001</v>
+        <v>-5.2344470000000003</v>
       </c>
       <c r="C2">
-        <v>0.85617580000000004</v>
+        <v>0.66532570000000002</v>
       </c>
       <c r="D2">
-        <v>-0.101775</v>
+        <v>-15.211919999999999</v>
       </c>
       <c r="E2">
-        <v>0.15206420000000001</v>
+        <v>16.83165</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -513,16 +516,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-5.6911350000000001</v>
+        <v>-5.2129599999999998</v>
       </c>
       <c r="C3">
-        <v>0.85617580000000004</v>
+        <v>1.223562</v>
       </c>
       <c r="D3">
-        <v>-0.101775</v>
+        <v>-0.12131550000000001</v>
       </c>
       <c r="E3">
-        <v>0.15206420000000001</v>
+        <v>0.19176019999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -530,16 +533,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-5.6911350000000001</v>
+        <v>-4.6287599999999998</v>
       </c>
       <c r="C4">
-        <v>0.85617580000000004</v>
+        <v>1.9464319999999999</v>
       </c>
       <c r="D4">
-        <v>-0.101775</v>
+        <v>-8.3843299999999996E-2</v>
       </c>
       <c r="E4">
-        <v>0.15206420000000001</v>
+        <v>0.22281899999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -547,16 +550,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-5.6911350000000001</v>
+        <v>-4.4178540000000002</v>
       </c>
       <c r="C5">
-        <v>0.85617580000000004</v>
+        <v>1.7649410000000001</v>
       </c>
       <c r="D5">
-        <v>-0.101775</v>
+        <v>1.10416E-2</v>
       </c>
       <c r="E5">
-        <v>0.15206420000000001</v>
+        <v>4.4161300000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -564,16 +567,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-5.6911350000000001</v>
+        <v>-4.2278710000000004</v>
       </c>
       <c r="C6">
-        <v>0.85617580000000004</v>
+        <v>3.007288</v>
       </c>
       <c r="D6">
-        <v>-0.101775</v>
+        <v>0.56911290000000003</v>
       </c>
       <c r="E6">
-        <v>0.15206420000000001</v>
+        <v>-0.34875349999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -581,16 +584,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-5.6911350000000001</v>
+        <v>-4.8775339999999998</v>
       </c>
       <c r="C7">
-        <v>0.85617580000000004</v>
+        <v>2.2744260000000001</v>
       </c>
       <c r="D7">
-        <v>-0.101775</v>
+        <v>-0.3779478</v>
       </c>
       <c r="E7">
-        <v>0.15206420000000001</v>
+        <v>1.01393</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -598,16 +601,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-5.6911350000000001</v>
+        <v>-3.8450220000000002</v>
       </c>
       <c r="C8">
-        <v>0.85617580000000004</v>
+        <v>2.1541239999999999</v>
       </c>
       <c r="D8">
-        <v>-0.101775</v>
+        <v>0.2284206</v>
       </c>
       <c r="E8">
-        <v>0.15206420000000001</v>
+        <v>-0.25769829999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -615,16 +618,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-5.6911350000000001</v>
+        <v>-4.7554369999999997</v>
       </c>
       <c r="C9">
-        <v>0.85617580000000004</v>
+        <v>2.3950550000000002</v>
       </c>
       <c r="D9">
-        <v>-0.101775</v>
+        <v>0.3886558</v>
       </c>
       <c r="E9">
-        <v>0.15206420000000001</v>
+        <v>-0.2791749</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -632,16 +635,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-5.6911350000000001</v>
+        <v>-5.6671630000000004</v>
       </c>
       <c r="C10">
-        <v>0.85617580000000004</v>
+        <v>4.0342339999999997</v>
       </c>
       <c r="D10">
-        <v>-0.101775</v>
+        <v>5.1410159999999996</v>
       </c>
       <c r="E10">
-        <v>0.15206420000000001</v>
+        <v>-1.3167120000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -649,16 +652,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-5.6911350000000001</v>
+        <v>-5.4756159999999996</v>
       </c>
       <c r="C11">
-        <v>0.85617580000000004</v>
+        <v>2.5759789999999998</v>
       </c>
       <c r="D11">
-        <v>-0.101775</v>
+        <v>0.52702470000000001</v>
       </c>
       <c r="E11">
-        <v>0.15206420000000001</v>
+        <v>-0.14951490000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -666,16 +669,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-5.6911350000000001</v>
+        <v>-4.8363240000000003</v>
       </c>
       <c r="C12">
-        <v>0.85617580000000004</v>
+        <v>2.1061580000000002</v>
       </c>
       <c r="D12">
-        <v>-0.101775</v>
+        <v>-6.8826E-3</v>
       </c>
       <c r="E12">
-        <v>0.15206420000000001</v>
+        <v>0.1339822</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -683,16 +686,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>-5.6911350000000001</v>
+        <v>-4.509239</v>
       </c>
       <c r="C13">
-        <v>0.85617580000000004</v>
+        <v>1.734809</v>
       </c>
       <c r="D13">
-        <v>-0.101775</v>
+        <v>1.66585E-2</v>
       </c>
       <c r="E13">
-        <v>0.15206420000000001</v>
+        <v>5.4263400000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -702,64 +705,900 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3244DEF6-B98C-4D05-8AEF-28F7E6CF6433}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.40691589</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.12712572</v>
+      </c>
+      <c r="C4">
+        <v>5.2938579999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-0.10955504000000001</v>
+      </c>
+      <c r="C5">
+        <v>-5.1988609999999998E-2</v>
+      </c>
+      <c r="D5">
+        <v>5.3624060000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>-9.8110459999999997E-2</v>
+      </c>
+      <c r="C6">
+        <v>-1.098056E-2</v>
+      </c>
+      <c r="D6">
+        <v>2.6486499999999998E-3</v>
+      </c>
+      <c r="E6">
+        <v>9.4377089999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>0.40691589</v>
+      </c>
+      <c r="C7">
+        <v>0.12712572</v>
+      </c>
+      <c r="D7">
+        <v>-0.10955504000000001</v>
+      </c>
+      <c r="E7">
+        <v>-9.8110459999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.40691589</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>0.12712572</v>
+      </c>
+      <c r="C8">
+        <v>5.2938579999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>-5.1988609999999998E-2</v>
+      </c>
+      <c r="E8">
+        <v>-1.098056E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.12712572</v>
+      </c>
+      <c r="G8">
+        <v>5.2938579999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-0.10955504000000001</v>
+      </c>
+      <c r="C9">
+        <v>-5.1988609999999998E-2</v>
+      </c>
+      <c r="D9">
+        <v>5.3624060000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>2.6486499999999998E-3</v>
+      </c>
+      <c r="F9">
+        <v>-0.10955504000000001</v>
+      </c>
+      <c r="G9">
+        <v>-5.1988609999999998E-2</v>
+      </c>
+      <c r="H9">
+        <v>5.3624060000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3965B3C-55A8-440B-BF8B-2678B86B5009}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>1.9475340999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>3.2511423000000002</v>
+      </c>
+      <c r="C4">
+        <v>6.2699214000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-0.94623522000000004</v>
+      </c>
+      <c r="C5">
+        <v>-2.0450987999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.72260157999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>-1.306141</v>
+      </c>
+      <c r="C6">
+        <v>-1.9828201999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.53938439999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.0090754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>1.9475340999999999</v>
+      </c>
+      <c r="C7">
+        <v>3.2511423000000002</v>
+      </c>
+      <c r="D7">
+        <v>-0.94623522000000004</v>
+      </c>
+      <c r="E7">
+        <v>-1.306141</v>
+      </c>
+      <c r="F7">
+        <v>1.9475340999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>3.2511423000000002</v>
+      </c>
+      <c r="C8">
+        <v>6.2699214000000003</v>
+      </c>
+      <c r="D8">
+        <v>-2.0450987999999999</v>
+      </c>
+      <c r="E8">
+        <v>-1.9828201999999999</v>
+      </c>
+      <c r="F8">
+        <v>3.2511423000000002</v>
+      </c>
+      <c r="G8">
+        <v>6.2699214000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-0.94623522000000004</v>
+      </c>
+      <c r="C9">
+        <v>-2.0450987999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.72260157999999997</v>
+      </c>
+      <c r="E9">
+        <v>0.53938439999999999</v>
+      </c>
+      <c r="F9">
+        <v>-0.94623522000000004</v>
+      </c>
+      <c r="G9">
+        <v>-2.0450987999999999</v>
+      </c>
+      <c r="H9">
+        <v>0.72260157999999997</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A36A1EC-6E83-42D1-8E16-DEA00F15C06D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>1.9900161000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2.7930595</v>
+      </c>
+      <c r="C4">
+        <v>5.0695813000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-2.4697398000000002</v>
+      </c>
+      <c r="C5">
+        <v>-4.6288476000000003</v>
+      </c>
+      <c r="D5">
+        <v>4.2416483999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>-1.1988524</v>
+      </c>
+      <c r="C6">
+        <v>-1.2920275999999999</v>
+      </c>
+      <c r="D6">
+        <v>1.0986727000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.95391148000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>1.9900161000000001</v>
+      </c>
+      <c r="C7">
+        <v>2.7930595</v>
+      </c>
+      <c r="D7">
+        <v>-2.4697398000000002</v>
+      </c>
+      <c r="E7">
+        <v>-1.1988524</v>
+      </c>
+      <c r="F7">
+        <v>1.9900161000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>2.7930595</v>
+      </c>
+      <c r="C8">
+        <v>5.0695813000000003</v>
+      </c>
+      <c r="D8">
+        <v>-4.6288476000000003</v>
+      </c>
+      <c r="E8">
+        <v>-1.2920275999999999</v>
+      </c>
+      <c r="F8">
+        <v>2.7930595</v>
+      </c>
+      <c r="G8">
+        <v>5.0695813000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-2.4697398000000002</v>
+      </c>
+      <c r="C9">
+        <v>-4.6288476000000003</v>
+      </c>
+      <c r="D9">
+        <v>4.2416483999999999</v>
+      </c>
+      <c r="E9">
+        <v>1.0986727000000001</v>
+      </c>
+      <c r="F9">
+        <v>-2.4697398000000002</v>
+      </c>
+      <c r="G9">
+        <v>-4.6288476000000003</v>
+      </c>
+      <c r="H9">
+        <v>4.2416483999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B898B43C-06D7-4D77-9CFF-D95B2C4C6A1D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.90014780999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.26880425000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.10679470000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-0.25028607000000003</v>
+      </c>
+      <c r="C5">
+        <v>-0.10724557999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.10953699</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0.20233461</v>
+      </c>
+      <c r="C6">
+        <v>0.10973328</v>
+      </c>
+      <c r="D6">
+        <v>-0.11460065</v>
+      </c>
+      <c r="E6">
+        <v>0.19922918000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>0.90014780999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.26880425000000002</v>
+      </c>
+      <c r="D7">
+        <v>-0.25028607000000003</v>
+      </c>
+      <c r="E7">
+        <v>0.20233461</v>
+      </c>
+      <c r="F7">
+        <v>0.90014780999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>0.26880425000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.10679470000000001</v>
+      </c>
+      <c r="D8">
+        <v>-0.10724557999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.10973328</v>
+      </c>
+      <c r="F8">
+        <v>0.26880425000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.10679470000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-0.25028607000000003</v>
+      </c>
+      <c r="C9">
+        <v>-0.10724557999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.10953699</v>
+      </c>
+      <c r="E9">
+        <v>-0.11460065</v>
+      </c>
+      <c r="F9">
+        <v>-0.25028607000000003</v>
+      </c>
+      <c r="G9">
+        <v>-0.10724557999999999</v>
+      </c>
+      <c r="H9">
+        <v>0.10953699</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916FC4D9-7F7F-4ABB-88CF-874043B3D3E6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection sqref="A1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.81329881999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.19434809</v>
+      </c>
+      <c r="C4">
+        <v>6.7213319999999993E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-0.20872035999999999</v>
+      </c>
+      <c r="C5">
+        <v>-8.1393400000000005E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.10161615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0.37428017000000002</v>
+      </c>
+      <c r="C6">
+        <v>0.13348182</v>
+      </c>
+      <c r="D6">
+        <v>-0.15895967</v>
+      </c>
+      <c r="E6">
+        <v>0.35530105000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>0.81329881999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.19434809</v>
+      </c>
+      <c r="D7">
+        <v>-0.20872035999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.37428017000000002</v>
+      </c>
+      <c r="F7">
+        <v>0.81329881999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>0.19434809</v>
+      </c>
+      <c r="C8">
+        <v>6.7213319999999993E-2</v>
+      </c>
+      <c r="D8">
+        <v>-8.1393400000000005E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.13348182</v>
+      </c>
+      <c r="F8">
+        <v>0.19434809</v>
+      </c>
+      <c r="G8">
+        <v>6.7213319999999993E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-0.20872035999999999</v>
+      </c>
+      <c r="C9">
+        <v>-8.1393400000000005E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.10161615</v>
+      </c>
+      <c r="E9">
+        <v>-0.15895967</v>
+      </c>
+      <c r="F9">
+        <v>-0.20872035999999999</v>
+      </c>
+      <c r="G9">
+        <v>-8.1393400000000005E-2</v>
+      </c>
+      <c r="H9">
+        <v>0.10161615</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -768,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8BE34F-251A-4B02-9EAF-7B6C81E08782}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -799,16 +1638,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-6.5937290191650302</v>
+        <v>-2.0087616443634002</v>
       </c>
       <c r="C2">
-        <v>0.51123619079589799</v>
+        <v>0.53235805034637396</v>
       </c>
       <c r="D2">
-        <v>1.3422158956527701</v>
+        <v>0.60818707942962602</v>
       </c>
       <c r="E2">
-        <v>2.8019282817840501</v>
+        <v>1.18028581142425</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -816,16 +1655,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-6.5937290191650302</v>
+        <v>-5.2074346542358398</v>
       </c>
       <c r="C3">
-        <v>0.51123619079589799</v>
+        <v>0.76891601085662797</v>
       </c>
       <c r="D3">
-        <v>1.3422158956527701</v>
+        <v>1.4988160133361801</v>
       </c>
       <c r="E3">
-        <v>2.8019282817840501</v>
+        <v>2.7222316265106201</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -833,16 +1672,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-6.5937290191650302</v>
+        <v>-3.01021027565002</v>
       </c>
       <c r="C4">
-        <v>0.51123619079589799</v>
+        <v>0.79645222425460804</v>
       </c>
       <c r="D4">
-        <v>1.3422158956527701</v>
+        <v>1.55413794517517</v>
       </c>
       <c r="E4">
-        <v>2.8019282817840501</v>
+        <v>2.5851204395294101</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -850,16 +1689,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-6.5937290191650302</v>
+        <v>-3.19253182411193</v>
       </c>
       <c r="C5">
-        <v>0.51123619079589799</v>
+        <v>0.77018427848815896</v>
       </c>
       <c r="D5">
-        <v>1.3422158956527701</v>
+        <v>1.56621742248535</v>
       </c>
       <c r="E5">
-        <v>2.8019282817840501</v>
+        <v>2.7048051357269198</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -867,16 +1706,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-6.5937290191650302</v>
+        <v>-1.1556499004364</v>
       </c>
       <c r="C6">
-        <v>0.51123619079589799</v>
+        <v>0.50794672966003396</v>
       </c>
       <c r="D6">
-        <v>1.3422158956527701</v>
+        <v>1.2501194477081301</v>
       </c>
       <c r="E6">
-        <v>2.8019282817840501</v>
+        <v>2.6661629676818799</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -884,16 +1723,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-6.5937290191650302</v>
+        <v>-0.73579609394073398</v>
       </c>
       <c r="C7">
-        <v>0.51123619079589799</v>
+        <v>0.105771109461784</v>
       </c>
       <c r="D7">
-        <v>1.3422158956527701</v>
+        <v>0.60967630147933904</v>
       </c>
       <c r="E7">
-        <v>2.8019282817840501</v>
+        <v>1.41994488239288</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -901,16 +1740,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-6.5937290191650302</v>
+        <v>-2.26299595832824</v>
       </c>
       <c r="C8">
-        <v>0.51123619079589799</v>
+        <v>0.50133514404296797</v>
       </c>
       <c r="D8">
-        <v>1.3422158956527701</v>
+        <v>1.7250130176544101</v>
       </c>
       <c r="E8">
-        <v>2.8019282817840501</v>
+        <v>2.6360216140746999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -918,16 +1757,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-6.5937290191650302</v>
+        <v>-1.0563949346542301</v>
       </c>
       <c r="C9">
-        <v>0.51123619079589799</v>
+        <v>0.76382696628570501</v>
       </c>
       <c r="D9">
-        <v>1.3422158956527701</v>
+        <v>1.5905055999755799</v>
       </c>
       <c r="E9">
-        <v>2.8019282817840501</v>
+        <v>2.6506259441375701</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -935,16 +1774,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-6.5937290191650302</v>
+        <v>0.27736204862594599</v>
       </c>
       <c r="C10">
-        <v>0.51123619079589799</v>
+        <v>0.55775624513626099</v>
       </c>
       <c r="D10">
-        <v>1.3422158956527701</v>
+        <v>1.3732042312621999</v>
       </c>
       <c r="E10">
-        <v>2.8019282817840501</v>
+        <v>2.2170286178588801</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -952,16 +1791,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-6.5937290191650302</v>
+        <v>-0.26222738623619002</v>
       </c>
       <c r="C11">
-        <v>0.51123619079589799</v>
+        <v>1.06166136264801</v>
       </c>
       <c r="D11">
-        <v>1.3422158956527701</v>
+        <v>1.2756724357604901</v>
       </c>
       <c r="E11">
-        <v>2.8019282817840501</v>
+        <v>2.5947744846343901</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -969,16 +1808,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-6.5937290191650302</v>
+        <v>-2.0087616443634002</v>
       </c>
       <c r="C12">
-        <v>0.51123619079589799</v>
+        <v>0.68005710840225198</v>
       </c>
       <c r="D12">
-        <v>1.3422158956527701</v>
+        <v>1.2625902891159</v>
       </c>
       <c r="E12">
-        <v>2.8019282817840501</v>
+        <v>2.6184096336364702</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1007,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E49F2D1-14B2-4EC2-9544-01485EF4F928}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1058,7 +1897,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>9.6792999999999998E-4</v>
+        <v>0.42047146000000002</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1066,10 +1905,10 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>9.7969999999999999E-5</v>
+        <v>1.2615064</v>
       </c>
       <c r="C4">
-        <v>1.9219999999999999E-5</v>
+        <v>71.131397000000007</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1077,13 +1916,13 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-1.1124E-4</v>
+        <v>-1.2937481</v>
       </c>
       <c r="C5">
-        <v>-2.493E-5</v>
+        <v>-78.024443000000005</v>
       </c>
       <c r="D5">
-        <v>3.2910000000000002E-5</v>
+        <v>85.607640000000004</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1091,16 +1930,16 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>1.9501399999999999E-3</v>
+        <v>0.18843132000000001</v>
       </c>
       <c r="C6">
-        <v>2.5813000000000002E-4</v>
+        <v>8.1101442000000006</v>
       </c>
       <c r="D6">
-        <v>-3.1076999999999998E-4</v>
+        <v>-8.8726929999999999</v>
       </c>
       <c r="E6">
-        <v>4.6216399999999998E-3</v>
+        <v>1.1692260999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1108,19 +1947,19 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>9.6792999999999998E-4</v>
+        <v>0.42047146000000002</v>
       </c>
       <c r="C7">
-        <v>9.7969999999999999E-5</v>
+        <v>1.2615064</v>
       </c>
       <c r="D7">
-        <v>-1.1124E-4</v>
+        <v>-1.2937481</v>
       </c>
       <c r="E7">
-        <v>1.9501399999999999E-3</v>
+        <v>0.18843132000000001</v>
       </c>
       <c r="F7">
-        <v>9.6792999999999998E-4</v>
+        <v>0.42047146000000002</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1128,22 +1967,22 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>9.7969999999999999E-5</v>
+        <v>1.2615064</v>
       </c>
       <c r="C8">
-        <v>1.9219999999999999E-5</v>
+        <v>71.131397000000007</v>
       </c>
       <c r="D8">
-        <v>-2.493E-5</v>
+        <v>-78.024443000000005</v>
       </c>
       <c r="E8">
-        <v>2.5813000000000002E-4</v>
+        <v>8.1101442000000006</v>
       </c>
       <c r="F8">
-        <v>9.7969999999999999E-5</v>
+        <v>1.2615064</v>
       </c>
       <c r="G8">
-        <v>1.9219999999999999E-5</v>
+        <v>71.131397000000007</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1151,22 +1990,22 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-1.1124E-4</v>
+        <v>-1.2937481</v>
       </c>
       <c r="C9">
-        <v>-2.493E-5</v>
+        <v>-78.024443000000005</v>
       </c>
       <c r="D9">
-        <v>3.2910000000000002E-5</v>
+        <v>85.607640000000004</v>
       </c>
       <c r="E9">
-        <v>-3.1076999999999998E-4</v>
+        <v>-8.8726929999999999</v>
       </c>
       <c r="F9">
-        <v>-1.1124E-4</v>
+        <v>-1.2937481</v>
       </c>
       <c r="G9">
-        <v>-2.493E-5</v>
+        <v>-78.024443000000005</v>
       </c>
     </row>
   </sheetData>
@@ -1176,74 +2015,1035 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38332D03-B727-46AC-AFEF-80C1DCAC7D58}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>5.5318279999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>7.43131E-3</v>
+      </c>
+      <c r="C4">
+        <v>1.65262E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-8.4337700000000002E-3</v>
+      </c>
+      <c r="C5">
+        <v>-2.1088299999999999E-3</v>
+      </c>
+      <c r="D5">
+        <v>2.7433700000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>7.4016620000000005E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.260929E-2</v>
+      </c>
+      <c r="D6">
+        <v>-1.51361E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.11819185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>5.5318279999999997E-2</v>
+      </c>
+      <c r="C7">
+        <v>7.43131E-3</v>
+      </c>
+      <c r="D7">
+        <v>-8.4337700000000002E-3</v>
+      </c>
+      <c r="E7">
+        <v>7.4016620000000005E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.5318279999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>7.43131E-3</v>
+      </c>
+      <c r="C8">
+        <v>1.65262E-3</v>
+      </c>
+      <c r="D8">
+        <v>-2.1088299999999999E-3</v>
+      </c>
+      <c r="E8">
+        <v>1.260929E-2</v>
+      </c>
+      <c r="F8">
+        <v>7.43131E-3</v>
+      </c>
+      <c r="G8">
+        <v>1.65262E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-8.4337700000000002E-3</v>
+      </c>
+      <c r="C9">
+        <v>-2.1088299999999999E-3</v>
+      </c>
+      <c r="D9">
+        <v>2.7433700000000002E-3</v>
+      </c>
+      <c r="E9">
+        <v>-1.51361E-2</v>
+      </c>
+      <c r="F9">
+        <v>-8.4337700000000002E-3</v>
+      </c>
+      <c r="G9">
+        <v>-2.1088299999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C3AE16-EB21-4284-99CF-0CA9218C00BB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.56969444999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.10252329</v>
+      </c>
+      <c r="C4">
+        <v>2.6091989999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-0.10939767</v>
+      </c>
+      <c r="C5">
+        <v>-3.1290480000000002E-2</v>
+      </c>
+      <c r="D5">
+        <v>3.8674159999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0.27300596999999999</v>
+      </c>
+      <c r="C6">
+        <v>7.3005249999999994E-2</v>
+      </c>
+      <c r="D6">
+        <v>-8.7417289999999995E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.24812039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>0.56969444999999996</v>
+      </c>
+      <c r="C7">
+        <v>0.10252329</v>
+      </c>
+      <c r="D7">
+        <v>-0.10939767</v>
+      </c>
+      <c r="E7">
+        <v>0.27300596999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.56969444999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>0.10252329</v>
+      </c>
+      <c r="C8">
+        <v>2.6091989999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>-3.1290480000000002E-2</v>
+      </c>
+      <c r="E8">
+        <v>7.3005249999999994E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.10252329</v>
+      </c>
+      <c r="G8">
+        <v>2.6091989999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-0.10939767</v>
+      </c>
+      <c r="C9">
+        <v>-3.1290480000000002E-2</v>
+      </c>
+      <c r="D9">
+        <v>3.8674159999999999E-2</v>
+      </c>
+      <c r="E9">
+        <v>-8.7417289999999995E-2</v>
+      </c>
+      <c r="F9">
+        <v>-0.10939767</v>
+      </c>
+      <c r="G9">
+        <v>-3.1290480000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6760BE32-F139-4EDF-B1ED-51D0BE4C1296}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>9.241104E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1.6527719999999999E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.5199000000000003E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-1.8061589999999999E-2</v>
+      </c>
+      <c r="C5">
+        <v>-5.6003600000000004E-3</v>
+      </c>
+      <c r="D5">
+        <v>7.13351E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>5.5314269999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.441041E-2</v>
+      </c>
+      <c r="D6">
+        <v>-1.7332859999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>5.7483449999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>9.241104E-2</v>
+      </c>
+      <c r="C7">
+        <v>1.6527719999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>-1.8061589999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>5.5314269999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>9.241104E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>1.6527719999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.5199000000000003E-3</v>
+      </c>
+      <c r="D8">
+        <v>-5.6003600000000004E-3</v>
+      </c>
+      <c r="E8">
+        <v>1.441041E-2</v>
+      </c>
+      <c r="F8">
+        <v>1.6527719999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>4.5199000000000003E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-1.8061589999999999E-2</v>
+      </c>
+      <c r="C9">
+        <v>-5.6003600000000004E-3</v>
+      </c>
+      <c r="D9">
+        <v>7.13351E-3</v>
+      </c>
+      <c r="E9">
+        <v>-1.7332859999999999E-2</v>
+      </c>
+      <c r="F9">
+        <v>-1.8061589999999999E-2</v>
+      </c>
+      <c r="G9">
+        <v>-5.6003600000000004E-3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B91EEF-CDAB-4F7B-ABA3-4E6266E86A22}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.70636441999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.22945457999999999</v>
+      </c>
+      <c r="C4">
+        <v>8.760954E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-0.17408932999999999</v>
+      </c>
+      <c r="C5">
+        <v>-7.1176409999999996E-2</v>
+      </c>
+      <c r="D5">
+        <v>5.9392920000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>-5.9708219999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.6188499999999998E-3</v>
+      </c>
+      <c r="D6">
+        <v>-8.2103000000000002E-3</v>
+      </c>
+      <c r="E6">
+        <v>8.3620609999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>0.70636441999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.22945457999999999</v>
+      </c>
+      <c r="D7">
+        <v>-0.17408932999999999</v>
+      </c>
+      <c r="E7">
+        <v>-5.9708219999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.70636441999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>0.22945457999999999</v>
+      </c>
+      <c r="C8">
+        <v>8.760954E-2</v>
+      </c>
+      <c r="D8">
+        <v>-7.1176409999999996E-2</v>
+      </c>
+      <c r="E8">
+        <v>2.6188499999999998E-3</v>
+      </c>
+      <c r="F8">
+        <v>0.22945457999999999</v>
+      </c>
+      <c r="G8">
+        <v>8.760954E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-0.17408932999999999</v>
+      </c>
+      <c r="C9">
+        <v>-7.1176409999999996E-2</v>
+      </c>
+      <c r="D9">
+        <v>5.9392920000000002E-2</v>
+      </c>
+      <c r="E9">
+        <v>-8.2103000000000002E-3</v>
+      </c>
+      <c r="F9">
+        <v>-0.17408932999999999</v>
+      </c>
+      <c r="G9">
+        <v>-7.1176409999999996E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6FA7F4-8E67-47E3-81E2-416898AAAC3B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>2.3806886</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2.2757955000000001</v>
+      </c>
+      <c r="C4">
+        <v>3.4321758999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-1.5834815</v>
+      </c>
+      <c r="C5">
+        <v>-2.8071348</v>
+      </c>
+      <c r="D5">
+        <v>2.3879427999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0.23198969999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.80907625000000005</v>
+      </c>
+      <c r="D6">
+        <v>-0.74656038999999996</v>
+      </c>
+      <c r="E6">
+        <v>0.45166137000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>2.3806886</v>
+      </c>
+      <c r="C7">
+        <v>2.2757955000000001</v>
+      </c>
+      <c r="D7">
+        <v>-1.5834815</v>
+      </c>
+      <c r="E7">
+        <v>0.23198969999999999</v>
+      </c>
+      <c r="F7">
+        <v>2.3806886</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>2.2757955000000001</v>
+      </c>
+      <c r="C8">
+        <v>3.4321758999999998</v>
+      </c>
+      <c r="D8">
+        <v>-2.8071348</v>
+      </c>
+      <c r="E8">
+        <v>0.80907625000000005</v>
+      </c>
+      <c r="F8">
+        <v>2.2757955000000001</v>
+      </c>
+      <c r="G8">
+        <v>3.4321758999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-1.5834815</v>
+      </c>
+      <c r="C9">
+        <v>-2.8071348</v>
+      </c>
+      <c r="D9">
+        <v>2.3879427999999998</v>
+      </c>
+      <c r="E9">
+        <v>-0.74656038999999996</v>
+      </c>
+      <c r="F9">
+        <v>-1.5834815</v>
+      </c>
+      <c r="G9">
+        <v>-2.8071348</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEED194A-5367-48BF-A33A-8A7BC8A330D8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.57527521999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>9.4986760000000003E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.1527379999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-0.1059372</v>
+      </c>
+      <c r="C5">
+        <v>-2.8231800000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>3.946761E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0.19848943999999999</v>
+      </c>
+      <c r="C6">
+        <v>5.1533509999999998E-2</v>
+      </c>
+      <c r="D6">
+        <v>-6.736955E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.21335344000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>0.57527521999999998</v>
+      </c>
+      <c r="C7">
+        <v>9.4986760000000003E-2</v>
+      </c>
+      <c r="D7">
+        <v>-0.1059372</v>
+      </c>
+      <c r="E7">
+        <v>0.19848943999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.57527521999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>9.4986760000000003E-2</v>
+      </c>
+      <c r="C8">
+        <v>2.1527379999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>-2.8231800000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>5.1533509999999998E-2</v>
+      </c>
+      <c r="F8">
+        <v>9.4986760000000003E-2</v>
+      </c>
+      <c r="G8">
+        <v>2.1527379999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-0.1059372</v>
+      </c>
+      <c r="C9">
+        <v>-2.8231800000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>3.946761E-2</v>
+      </c>
+      <c r="E9">
+        <v>-6.736955E-2</v>
+      </c>
+      <c r="F9">
+        <v>-0.1059372</v>
+      </c>
+      <c r="G9">
+        <v>-2.8231800000000001E-2</v>
+      </c>
+      <c r="H9">
+        <v>3.946761E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated data on spline models
</commit_message>
<xml_diff>
--- a/data/55-64_Female_first_revision.xlsx
+++ b/data/55-64_Female_first_revision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/KNIPS/code/KNIPS-Semi-Markov/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB6B13B1-8800-45EC-8B41-9ED86E8D1DB5}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E234CD4E-6FE2-4C48-B089-81DE901C8A54}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rcs_first_revision_mean" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="37">
   <si>
     <t>bound1</t>
   </si>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -499,16 +499,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-5.2344470000000003</v>
+        <v>-6.7902209999999998</v>
       </c>
       <c r="C2">
-        <v>0.66532570000000002</v>
+        <v>0.2437356</v>
       </c>
       <c r="D2">
-        <v>-15.211919999999999</v>
+        <v>-0.1136004</v>
       </c>
       <c r="E2">
-        <v>16.83165</v>
+        <v>0.20844499999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -516,16 +516,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-5.2129599999999998</v>
+        <v>-4.7206780000000004</v>
       </c>
       <c r="C3">
-        <v>1.223562</v>
+        <v>1.4803789999999999</v>
       </c>
       <c r="D3">
-        <v>-0.12131550000000001</v>
+        <v>-7.7839000000000005E-2</v>
       </c>
       <c r="E3">
-        <v>0.19176019999999999</v>
+        <v>0.136932</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -533,16 +533,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-4.6287599999999998</v>
+        <v>-4.7926880000000001</v>
       </c>
       <c r="C4">
-        <v>1.9464319999999999</v>
+        <v>1.626582</v>
       </c>
       <c r="D4">
-        <v>-8.3843299999999996E-2</v>
+        <v>-4.1035599999999998E-2</v>
       </c>
       <c r="E4">
-        <v>0.22281899999999999</v>
+        <v>0.121294</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -550,16 +550,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-4.4178540000000002</v>
+        <v>-6.1213220000000002</v>
       </c>
       <c r="C5">
-        <v>1.7649410000000001</v>
+        <v>0.79234680000000002</v>
       </c>
       <c r="D5">
-        <v>1.10416E-2</v>
+        <v>-0.22510720000000001</v>
       </c>
       <c r="E5">
-        <v>4.4161300000000001E-2</v>
+        <v>0.32448189999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -567,16 +567,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-4.2278710000000004</v>
+        <v>-5.6073170000000001</v>
       </c>
       <c r="C6">
-        <v>3.007288</v>
+        <v>1.0214510000000001</v>
       </c>
       <c r="D6">
-        <v>0.56911290000000003</v>
+        <v>-0.19340070000000001</v>
       </c>
       <c r="E6">
-        <v>-0.34875349999999999</v>
+        <v>0.3403776</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -584,16 +584,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-4.8775339999999998</v>
+        <v>-4.8346359999999997</v>
       </c>
       <c r="C7">
-        <v>2.2744260000000001</v>
+        <v>0.97691830000000002</v>
       </c>
       <c r="D7">
-        <v>-0.3779478</v>
+        <v>7.1402400000000005E-2</v>
       </c>
       <c r="E7">
-        <v>1.01393</v>
+        <v>-8.4301699999999993E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -601,16 +601,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-3.8450220000000002</v>
+        <v>-3.347934</v>
       </c>
       <c r="C8">
-        <v>2.1541239999999999</v>
+        <v>2.5355379999999998</v>
       </c>
       <c r="D8">
-        <v>0.2284206</v>
+        <v>0.1602712</v>
       </c>
       <c r="E8">
-        <v>-0.25769829999999999</v>
+        <v>-0.146985</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -618,16 +618,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-4.7554369999999997</v>
+        <v>-4.6625620000000003</v>
       </c>
       <c r="C9">
-        <v>2.3950550000000002</v>
+        <v>1.946941</v>
       </c>
       <c r="D9">
-        <v>0.3886558</v>
+        <v>2.2343700000000001E-2</v>
       </c>
       <c r="E9">
-        <v>-0.2791749</v>
+        <v>6.3308500000000004E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -635,16 +635,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-5.6671630000000004</v>
+        <v>-4.8020569999999996</v>
       </c>
       <c r="C10">
-        <v>4.0342339999999997</v>
+        <v>1.8921619999999999</v>
       </c>
       <c r="D10">
-        <v>5.1410159999999996</v>
+        <v>0.45438909999999999</v>
       </c>
       <c r="E10">
-        <v>-1.3167120000000001</v>
+        <v>-0.69997430000000005</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -652,16 +652,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-5.4756159999999996</v>
+        <v>-4.9300420000000003</v>
       </c>
       <c r="C11">
-        <v>2.5759789999999998</v>
+        <v>1.8155559999999999</v>
       </c>
       <c r="D11">
-        <v>0.52702470000000001</v>
+        <v>0.1690354</v>
       </c>
       <c r="E11">
-        <v>-0.14951490000000001</v>
+        <v>-2.08904E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -669,16 +669,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-4.8363240000000003</v>
+        <v>-5.6909530000000004</v>
       </c>
       <c r="C12">
-        <v>2.1061580000000002</v>
+        <v>2.4107090000000002</v>
       </c>
       <c r="D12">
-        <v>-6.8826E-3</v>
+        <v>0.37093179999999998</v>
       </c>
       <c r="E12">
-        <v>0.1339822</v>
+        <v>-0.2498243</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -686,16 +686,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>-4.509239</v>
+        <v>-4.9340789999999997</v>
       </c>
       <c r="C13">
-        <v>1.734809</v>
+        <v>0.62195080000000003</v>
       </c>
       <c r="D13">
-        <v>1.66585E-2</v>
+        <v>-0.17890510000000001</v>
       </c>
       <c r="E13">
-        <v>5.4263400000000003E-2</v>
+        <v>0.27540300000000001</v>
       </c>
     </row>
   </sheetData>
@@ -764,7 +764,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>0.40691589</v>
+        <v>0.26684126000000002</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -772,10 +772,10 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>0.12712572</v>
+        <v>4.856224E-2</v>
       </c>
       <c r="C4">
-        <v>5.2938579999999999E-2</v>
+        <v>1.239874E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -783,13 +783,13 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-0.10955504000000001</v>
+        <v>-4.8386480000000003E-2</v>
       </c>
       <c r="C5">
-        <v>-5.1988609999999998E-2</v>
+        <v>-1.383994E-2</v>
       </c>
       <c r="D5">
-        <v>5.3624060000000001E-2</v>
+        <v>1.5916489999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -797,16 +797,16 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>-9.8110459999999997E-2</v>
+        <v>0.11553550999999999</v>
       </c>
       <c r="C6">
-        <v>-1.098056E-2</v>
+        <v>3.2168229999999999E-2</v>
       </c>
       <c r="D6">
-        <v>2.6486499999999998E-3</v>
+        <v>-3.6001239999999997E-2</v>
       </c>
       <c r="E6">
-        <v>9.4377089999999997E-2</v>
+        <v>0.11112564</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -814,19 +814,19 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>0.40691589</v>
+        <v>0.26684126000000002</v>
       </c>
       <c r="C7">
-        <v>0.12712572</v>
+        <v>4.856224E-2</v>
       </c>
       <c r="D7">
-        <v>-0.10955504000000001</v>
+        <v>-4.8386480000000003E-2</v>
       </c>
       <c r="E7">
-        <v>-9.8110459999999997E-2</v>
+        <v>0.11553550999999999</v>
       </c>
       <c r="F7">
-        <v>0.40691589</v>
+        <v>0.26684126000000002</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -834,22 +834,22 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>0.12712572</v>
+        <v>4.856224E-2</v>
       </c>
       <c r="C8">
-        <v>5.2938579999999999E-2</v>
+        <v>1.239874E-2</v>
       </c>
       <c r="D8">
-        <v>-5.1988609999999998E-2</v>
+        <v>-1.383994E-2</v>
       </c>
       <c r="E8">
-        <v>-1.098056E-2</v>
+        <v>3.2168229999999999E-2</v>
       </c>
       <c r="F8">
-        <v>0.12712572</v>
+        <v>4.856224E-2</v>
       </c>
       <c r="G8">
-        <v>5.2938579999999999E-2</v>
+        <v>1.239874E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -857,25 +857,25 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-0.10955504000000001</v>
+        <v>-4.8386480000000003E-2</v>
       </c>
       <c r="C9">
-        <v>-5.1988609999999998E-2</v>
+        <v>-1.383994E-2</v>
       </c>
       <c r="D9">
-        <v>5.3624060000000001E-2</v>
+        <v>1.5916489999999998E-2</v>
       </c>
       <c r="E9">
-        <v>2.6486499999999998E-3</v>
+        <v>-3.6001239999999997E-2</v>
       </c>
       <c r="F9">
-        <v>-0.10955504000000001</v>
+        <v>-4.8386480000000003E-2</v>
       </c>
       <c r="G9">
-        <v>-5.1988609999999998E-2</v>
+        <v>-1.383994E-2</v>
       </c>
       <c r="H9">
-        <v>5.3624060000000001E-2</v>
+        <v>1.5916489999999998E-2</v>
       </c>
     </row>
   </sheetData>
@@ -944,7 +944,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>1.9475340999999999</v>
+        <v>0.42092476000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -952,10 +952,10 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>3.2511423000000002</v>
+        <v>0.13039955</v>
       </c>
       <c r="C4">
-        <v>6.2699214000000003</v>
+        <v>6.8574570000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -963,13 +963,13 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-0.94623522000000004</v>
+        <v>-0.15346371</v>
       </c>
       <c r="C5">
-        <v>-2.0450987999999999</v>
+        <v>-0.10817918999999999</v>
       </c>
       <c r="D5">
-        <v>0.72260157999999997</v>
+        <v>0.18926403</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -977,16 +977,16 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>-1.306141</v>
+        <v>-0.20475419</v>
       </c>
       <c r="C6">
-        <v>-1.9828201999999999</v>
+        <v>-3.0850949999999999E-2</v>
       </c>
       <c r="D6">
-        <v>0.53938439999999999</v>
+        <v>1.8272679999999999E-2</v>
       </c>
       <c r="E6">
-        <v>1.0090754</v>
+        <v>0.23435366999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -994,19 +994,19 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>1.9475340999999999</v>
+        <v>0.42092476000000001</v>
       </c>
       <c r="C7">
-        <v>3.2511423000000002</v>
+        <v>0.13039955</v>
       </c>
       <c r="D7">
-        <v>-0.94623522000000004</v>
+        <v>-0.15346371</v>
       </c>
       <c r="E7">
-        <v>-1.306141</v>
+        <v>-0.20475419</v>
       </c>
       <c r="F7">
-        <v>1.9475340999999999</v>
+        <v>0.42092476000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1014,22 +1014,22 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>3.2511423000000002</v>
+        <v>0.13039955</v>
       </c>
       <c r="C8">
-        <v>6.2699214000000003</v>
+        <v>6.8574570000000001E-2</v>
       </c>
       <c r="D8">
-        <v>-2.0450987999999999</v>
+        <v>-0.10817918999999999</v>
       </c>
       <c r="E8">
-        <v>-1.9828201999999999</v>
+        <v>-3.0850949999999999E-2</v>
       </c>
       <c r="F8">
-        <v>3.2511423000000002</v>
+        <v>0.13039955</v>
       </c>
       <c r="G8">
-        <v>6.2699214000000003</v>
+        <v>6.8574570000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1037,25 +1037,25 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-0.94623522000000004</v>
+        <v>-0.15346371</v>
       </c>
       <c r="C9">
-        <v>-2.0450987999999999</v>
+        <v>-0.10817918999999999</v>
       </c>
       <c r="D9">
-        <v>0.72260157999999997</v>
+        <v>0.18926403</v>
       </c>
       <c r="E9">
-        <v>0.53938439999999999</v>
+        <v>1.8272679999999999E-2</v>
       </c>
       <c r="F9">
-        <v>-0.94623522000000004</v>
+        <v>-0.15346371</v>
       </c>
       <c r="G9">
-        <v>-2.0450987999999999</v>
+        <v>-0.10817918999999999</v>
       </c>
       <c r="H9">
-        <v>0.72260157999999997</v>
+        <v>0.18926403</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1068,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H9"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1124,7 +1124,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>1.9900161000000001</v>
+        <v>0.39678466000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1132,10 +1132,10 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>2.7930595</v>
+        <v>0.1269129</v>
       </c>
       <c r="C4">
-        <v>5.0695813000000003</v>
+        <v>6.1192919999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1143,13 +1143,13 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-2.4697398000000002</v>
+        <v>-0.10831236</v>
       </c>
       <c r="C5">
-        <v>-4.6288476000000003</v>
+        <v>-6.2812960000000001E-2</v>
       </c>
       <c r="D5">
-        <v>4.2416483999999999</v>
+        <v>6.8450730000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1157,16 +1157,16 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>-1.1988524</v>
+        <v>-9.9675200000000005E-2</v>
       </c>
       <c r="C6">
-        <v>-1.2920275999999999</v>
+        <v>3.1674199999999998E-3</v>
       </c>
       <c r="D6">
-        <v>1.0986727000000001</v>
+        <v>-1.7227369999999999E-2</v>
       </c>
       <c r="E6">
-        <v>0.95391148000000003</v>
+        <v>0.14591982000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1174,19 +1174,19 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>1.9900161000000001</v>
+        <v>0.39678466000000001</v>
       </c>
       <c r="C7">
-        <v>2.7930595</v>
+        <v>0.1269129</v>
       </c>
       <c r="D7">
-        <v>-2.4697398000000002</v>
+        <v>-0.10831236</v>
       </c>
       <c r="E7">
-        <v>-1.1988524</v>
+        <v>-9.9675200000000005E-2</v>
       </c>
       <c r="F7">
-        <v>1.9900161000000001</v>
+        <v>0.39678466000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1194,22 +1194,22 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>2.7930595</v>
+        <v>0.1269129</v>
       </c>
       <c r="C8">
-        <v>5.0695813000000003</v>
+        <v>6.1192919999999998E-2</v>
       </c>
       <c r="D8">
-        <v>-4.6288476000000003</v>
+        <v>-6.2812960000000001E-2</v>
       </c>
       <c r="E8">
-        <v>-1.2920275999999999</v>
+        <v>3.1674199999999998E-3</v>
       </c>
       <c r="F8">
-        <v>2.7930595</v>
+        <v>0.1269129</v>
       </c>
       <c r="G8">
-        <v>5.0695813000000003</v>
+        <v>6.1192919999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1217,25 +1217,25 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-2.4697398000000002</v>
+        <v>-0.10831236</v>
       </c>
       <c r="C9">
-        <v>-4.6288476000000003</v>
+        <v>-6.2812960000000001E-2</v>
       </c>
       <c r="D9">
-        <v>4.2416483999999999</v>
+        <v>6.8450730000000001E-2</v>
       </c>
       <c r="E9">
-        <v>1.0986727000000001</v>
+        <v>-1.7227369999999999E-2</v>
       </c>
       <c r="F9">
-        <v>-2.4697398000000002</v>
+        <v>-0.10831236</v>
       </c>
       <c r="G9">
-        <v>-4.6288476000000003</v>
+        <v>-6.2812960000000001E-2</v>
       </c>
       <c r="H9">
-        <v>4.2416483999999999</v>
+        <v>6.8450730000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1248,7 +1248,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1304,7 +1304,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>0.90014780999999999</v>
+        <v>0.54043713999999998</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1312,10 +1312,10 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>0.26880425000000002</v>
+        <v>0.19312313</v>
       </c>
       <c r="C4">
-        <v>0.10679470000000001</v>
+        <v>9.561248E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1323,13 +1323,13 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-0.25028607000000003</v>
+        <v>-0.17131499</v>
       </c>
       <c r="C5">
-        <v>-0.10724557999999999</v>
+        <v>-9.582359E-2</v>
       </c>
       <c r="D5">
-        <v>0.10953699</v>
+        <v>9.9665630000000005E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1337,16 +1337,16 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>0.20233461</v>
+        <v>-8.6726339999999999E-2</v>
       </c>
       <c r="C6">
-        <v>0.10973328</v>
+        <v>2.6263300000000001E-3</v>
       </c>
       <c r="D6">
-        <v>-0.11460065</v>
+        <v>-1.293425E-2</v>
       </c>
       <c r="E6">
-        <v>0.19922918000000001</v>
+        <v>0.10757497000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1354,19 +1354,19 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>0.90014780999999999</v>
+        <v>0.54043713999999998</v>
       </c>
       <c r="C7">
-        <v>0.26880425000000002</v>
+        <v>0.19312313</v>
       </c>
       <c r="D7">
-        <v>-0.25028607000000003</v>
+        <v>-0.17131499</v>
       </c>
       <c r="E7">
-        <v>0.20233461</v>
+        <v>-8.6726339999999999E-2</v>
       </c>
       <c r="F7">
-        <v>0.90014780999999999</v>
+        <v>0.54043713999999998</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1374,22 +1374,22 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>0.26880425000000002</v>
+        <v>0.19312313</v>
       </c>
       <c r="C8">
-        <v>0.10679470000000001</v>
+        <v>9.561248E-2</v>
       </c>
       <c r="D8">
-        <v>-0.10724557999999999</v>
+        <v>-9.582359E-2</v>
       </c>
       <c r="E8">
-        <v>0.10973328</v>
+        <v>2.6263300000000001E-3</v>
       </c>
       <c r="F8">
-        <v>0.26880425000000002</v>
+        <v>0.19312313</v>
       </c>
       <c r="G8">
-        <v>0.10679470000000001</v>
+        <v>9.561248E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1397,25 +1397,25 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-0.25028607000000003</v>
+        <v>-0.17131499</v>
       </c>
       <c r="C9">
-        <v>-0.10724557999999999</v>
+        <v>-9.582359E-2</v>
       </c>
       <c r="D9">
-        <v>0.10953699</v>
+        <v>9.9665630000000005E-2</v>
       </c>
       <c r="E9">
-        <v>-0.11460065</v>
+        <v>-1.293425E-2</v>
       </c>
       <c r="F9">
-        <v>-0.25028607000000003</v>
+        <v>-0.17131499</v>
       </c>
       <c r="G9">
-        <v>-0.10724557999999999</v>
+        <v>-9.582359E-2</v>
       </c>
       <c r="H9">
-        <v>0.10953699</v>
+        <v>9.9665630000000005E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1425,6 +1425,799 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916FC4D9-7F7F-4ABB-88CF-874043B3D3E6}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>5.8394719999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1.0862719999999999E-2</v>
+      </c>
+      <c r="C4">
+        <v>8.5972500000000007E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-1.233916E-2</v>
+      </c>
+      <c r="C5">
+        <v>-1.276822E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.9354340000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>5.4121820000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>3.1502120000000002E-2</v>
+      </c>
+      <c r="D6">
+        <v>-4.3857599999999997E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.17889764</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>5.8394719999999997E-2</v>
+      </c>
+      <c r="C7">
+        <v>1.0862719999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>-1.233916E-2</v>
+      </c>
+      <c r="E7">
+        <v>5.4121820000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.8394719999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>1.0862719999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>8.5972500000000007E-3</v>
+      </c>
+      <c r="D8">
+        <v>-1.276822E-2</v>
+      </c>
+      <c r="E8">
+        <v>3.1502120000000002E-2</v>
+      </c>
+      <c r="F8">
+        <v>1.0862719999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>8.5972500000000007E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-1.233916E-2</v>
+      </c>
+      <c r="C9">
+        <v>-1.276822E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.9354340000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>-4.3857599999999997E-2</v>
+      </c>
+      <c r="F9">
+        <v>-1.233916E-2</v>
+      </c>
+      <c r="G9">
+        <v>-1.276822E-2</v>
+      </c>
+      <c r="H9">
+        <v>1.9354340000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8BE34F-251A-4B02-9EAF-7B6C81E08782}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="27.83984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>-6.5937290191650302</v>
+      </c>
+      <c r="C2">
+        <v>0.35132184624671903</v>
+      </c>
+      <c r="D2">
+        <v>1.3683381080627399</v>
+      </c>
+      <c r="E2">
+        <v>2.1021120548248202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>-6.5937290191650302</v>
+      </c>
+      <c r="C3">
+        <v>0.62003910541534402</v>
+      </c>
+      <c r="D3">
+        <v>1.3978630304336499</v>
+      </c>
+      <c r="E3">
+        <v>2.7754933834075901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>-3.95467185974121</v>
+      </c>
+      <c r="C4">
+        <v>0.93460255861282304</v>
+      </c>
+      <c r="D4">
+        <v>1.7186514139175399</v>
+      </c>
+      <c r="E4">
+        <v>2.72922539710998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>-6.5937290191650302</v>
+      </c>
+      <c r="C5">
+        <v>0.73405128717422397</v>
+      </c>
+      <c r="D5">
+        <v>1.4480054378509499</v>
+      </c>
+      <c r="E5">
+        <v>2.7851717472076398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>-4.2911443710327104</v>
+      </c>
+      <c r="C6">
+        <v>0.88838970661163297</v>
+      </c>
+      <c r="D6">
+        <v>1.70779240131378</v>
+      </c>
+      <c r="E6">
+        <v>2.6451985836028999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>-2.95614314079284</v>
+      </c>
+      <c r="C7">
+        <v>0.105771109461784</v>
+      </c>
+      <c r="D7">
+        <v>0.931371510028839</v>
+      </c>
+      <c r="E7">
+        <v>2.4115531444549498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>-3.5026867389678902</v>
+      </c>
+      <c r="C8">
+        <v>0.57946252822875899</v>
+      </c>
+      <c r="D8">
+        <v>1.6872351169586099</v>
+      </c>
+      <c r="E8">
+        <v>2.6535215377807599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>-2.7650878429412802</v>
+      </c>
+      <c r="C9">
+        <v>0.70606815814971902</v>
+      </c>
+      <c r="D9">
+        <v>1.4809198379516599</v>
+      </c>
+      <c r="E9">
+        <v>2.6937572956085201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>-0.73579609394073398</v>
+      </c>
+      <c r="C10">
+        <v>0.952717065811157</v>
+      </c>
+      <c r="D10">
+        <v>2.0424907207489</v>
+      </c>
+      <c r="E10">
+        <v>2.5960001945495601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>-0.95893961191177302</v>
+      </c>
+      <c r="C11">
+        <v>0.70876717567443803</v>
+      </c>
+      <c r="D11">
+        <v>1.59662520885467</v>
+      </c>
+      <c r="E11">
+        <v>2.5343158245086599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>-1.1384080648422199</v>
+      </c>
+      <c r="C12">
+        <v>0.74840247631072998</v>
+      </c>
+      <c r="D12">
+        <v>1.45952188968658</v>
+      </c>
+      <c r="E12">
+        <v>2.5390820503234801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>-3.3356328010559002</v>
+      </c>
+      <c r="C13">
+        <v>0.423776924610137</v>
+      </c>
+      <c r="D13">
+        <v>1.27720034122467</v>
+      </c>
+      <c r="E13">
+        <v>2.2933709621429399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16">
+        <v>-3.3356328010559002</v>
+      </c>
+      <c r="D16">
+        <v>0.423776924610137</v>
+      </c>
+      <c r="E16">
+        <v>1.27720034122467</v>
+      </c>
+      <c r="F16">
+        <v>2.2933709621429399</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E49F2D1-14B2-4EC2-9544-01485EF4F928}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>5.736513E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>5.9890200000000003E-3</v>
+      </c>
+      <c r="C4">
+        <v>1.549818E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-9.3747799999999992E-3</v>
+      </c>
+      <c r="C5">
+        <v>-3.3792709999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>7.4097389999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0.12364248999999999</v>
+      </c>
+      <c r="C6">
+        <v>9.9479300000000007E-2</v>
+      </c>
+      <c r="D6">
+        <v>-0.20307086999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.2193856000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>5.736513E-2</v>
+      </c>
+      <c r="C7">
+        <v>5.9890200000000003E-3</v>
+      </c>
+      <c r="D7">
+        <v>-9.3747799999999992E-3</v>
+      </c>
+      <c r="E7">
+        <v>0.12364248999999999</v>
+      </c>
+      <c r="F7">
+        <v>5.736513E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>5.9890200000000003E-3</v>
+      </c>
+      <c r="C8">
+        <v>1.549818E-2</v>
+      </c>
+      <c r="D8">
+        <v>-3.3792709999999997E-2</v>
+      </c>
+      <c r="E8">
+        <v>9.9479300000000007E-2</v>
+      </c>
+      <c r="F8">
+        <v>5.9890200000000003E-3</v>
+      </c>
+      <c r="G8">
+        <v>1.549818E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-9.3747799999999992E-3</v>
+      </c>
+      <c r="C9">
+        <v>-3.3792709999999997E-2</v>
+      </c>
+      <c r="D9">
+        <v>7.4097389999999999E-2</v>
+      </c>
+      <c r="E9">
+        <v>-0.20307086999999999</v>
+      </c>
+      <c r="F9">
+        <v>-9.3747799999999992E-3</v>
+      </c>
+      <c r="G9">
+        <v>-3.3792709999999997E-2</v>
+      </c>
+      <c r="H9">
+        <v>7.4097389999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38332D03-B727-46AC-AFEF-80C1DCAC7D58}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>2.7788739999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2.71712E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.9777999999999998E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-3.0265399999999999E-3</v>
+      </c>
+      <c r="C5">
+        <v>-4.9023999999999997E-4</v>
+      </c>
+      <c r="D5">
+        <v>6.1576999999999997E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>5.1944740000000003E-2</v>
+      </c>
+      <c r="C6">
+        <v>5.8794399999999997E-3</v>
+      </c>
+      <c r="D6">
+        <v>-6.8030199999999999E-3</v>
+      </c>
+      <c r="E6">
+        <v>0.10532962999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>2.7788739999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>2.71712E-3</v>
+      </c>
+      <c r="D7">
+        <v>-3.0265399999999999E-3</v>
+      </c>
+      <c r="E7">
+        <v>5.1944740000000003E-2</v>
+      </c>
+      <c r="F7">
+        <v>2.7788739999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>2.71712E-3</v>
+      </c>
+      <c r="C8">
+        <v>3.9777999999999998E-4</v>
+      </c>
+      <c r="D8">
+        <v>-4.9023999999999997E-4</v>
+      </c>
+      <c r="E8">
+        <v>5.8794399999999997E-3</v>
+      </c>
+      <c r="F8">
+        <v>2.71712E-3</v>
+      </c>
+      <c r="G8">
+        <v>3.9777999999999998E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>-3.0265399999999999E-3</v>
+      </c>
+      <c r="C9">
+        <v>-4.9023999999999997E-4</v>
+      </c>
+      <c r="D9">
+        <v>6.1576999999999997E-4</v>
+      </c>
+      <c r="E9">
+        <v>-6.8030199999999999E-3</v>
+      </c>
+      <c r="F9">
+        <v>-3.0265399999999999E-3</v>
+      </c>
+      <c r="G9">
+        <v>-4.9023999999999997E-4</v>
+      </c>
+      <c r="H9">
+        <v>6.1576999999999997E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C3AE16-EB21-4284-99CF-0CA9218C00BB}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1484,7 +2277,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>0.81329881999999998</v>
+        <v>0.18013306000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1492,10 +2285,10 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>0.19434809</v>
+        <v>2.728887E-2</v>
       </c>
       <c r="C4">
-        <v>6.7213319999999993E-2</v>
+        <v>6.4815599999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1503,13 +2296,13 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-0.20872035999999999</v>
+        <v>-3.1784739999999999E-2</v>
       </c>
       <c r="C5">
-        <v>-8.1393400000000005E-2</v>
+        <v>-8.6093999999999997E-3</v>
       </c>
       <c r="D5">
-        <v>0.10161615</v>
+        <v>1.1756020000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1517,16 +2310,16 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>0.37428017000000002</v>
+        <v>0.13799523999999999</v>
       </c>
       <c r="C6">
-        <v>0.13348182</v>
+        <v>2.916034E-2</v>
       </c>
       <c r="D6">
-        <v>-0.15895967</v>
+        <v>-3.7147310000000003E-2</v>
       </c>
       <c r="E6">
-        <v>0.35530105000000001</v>
+        <v>0.15891043999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1534,19 +2327,19 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>0.81329881999999998</v>
+        <v>0.18013306000000001</v>
       </c>
       <c r="C7">
-        <v>0.19434809</v>
+        <v>2.728887E-2</v>
       </c>
       <c r="D7">
-        <v>-0.20872035999999999</v>
+        <v>-3.1784739999999999E-2</v>
       </c>
       <c r="E7">
-        <v>0.37428017000000002</v>
+        <v>0.13799523999999999</v>
       </c>
       <c r="F7">
-        <v>0.81329881999999998</v>
+        <v>0.18013306000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1554,22 +2347,22 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>0.19434809</v>
+        <v>2.728887E-2</v>
       </c>
       <c r="C8">
-        <v>6.7213319999999993E-2</v>
+        <v>6.4815599999999999E-3</v>
       </c>
       <c r="D8">
-        <v>-8.1393400000000005E-2</v>
+        <v>-8.6093999999999997E-3</v>
       </c>
       <c r="E8">
-        <v>0.13348182</v>
+        <v>2.916034E-2</v>
       </c>
       <c r="F8">
-        <v>0.19434809</v>
+        <v>2.728887E-2</v>
       </c>
       <c r="G8">
-        <v>6.7213319999999993E-2</v>
+        <v>6.4815599999999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1577,777 +2370,25 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-0.20872035999999999</v>
+        <v>-3.1784739999999999E-2</v>
       </c>
       <c r="C9">
-        <v>-8.1393400000000005E-2</v>
+        <v>-8.6093999999999997E-3</v>
       </c>
       <c r="D9">
-        <v>0.10161615</v>
+        <v>1.1756020000000001E-2</v>
       </c>
       <c r="E9">
-        <v>-0.15895967</v>
+        <v>-3.7147310000000003E-2</v>
       </c>
       <c r="F9">
-        <v>-0.20872035999999999</v>
+        <v>-3.1784739999999999E-2</v>
       </c>
       <c r="G9">
-        <v>-8.1393400000000005E-2</v>
+        <v>-8.6093999999999997E-3</v>
       </c>
       <c r="H9">
-        <v>0.10161615</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8BE34F-251A-4B02-9EAF-7B6C81E08782}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="27.83984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>-2.0087616443634002</v>
-      </c>
-      <c r="C2">
-        <v>0.53235805034637396</v>
-      </c>
-      <c r="D2">
-        <v>0.60818707942962602</v>
-      </c>
-      <c r="E2">
-        <v>1.18028581142425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>-5.2074346542358398</v>
-      </c>
-      <c r="C3">
-        <v>0.76891601085662797</v>
-      </c>
-      <c r="D3">
-        <v>1.4988160133361801</v>
-      </c>
-      <c r="E3">
-        <v>2.7222316265106201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>-3.01021027565002</v>
-      </c>
-      <c r="C4">
-        <v>0.79645222425460804</v>
-      </c>
-      <c r="D4">
-        <v>1.55413794517517</v>
-      </c>
-      <c r="E4">
-        <v>2.5851204395294101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>-3.19253182411193</v>
-      </c>
-      <c r="C5">
-        <v>0.77018427848815896</v>
-      </c>
-      <c r="D5">
-        <v>1.56621742248535</v>
-      </c>
-      <c r="E5">
-        <v>2.7048051357269198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>-1.1556499004364</v>
-      </c>
-      <c r="C6">
-        <v>0.50794672966003396</v>
-      </c>
-      <c r="D6">
-        <v>1.2501194477081301</v>
-      </c>
-      <c r="E6">
-        <v>2.6661629676818799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>-0.73579609394073398</v>
-      </c>
-      <c r="C7">
-        <v>0.105771109461784</v>
-      </c>
-      <c r="D7">
-        <v>0.60967630147933904</v>
-      </c>
-      <c r="E7">
-        <v>1.41994488239288</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>-2.26299595832824</v>
-      </c>
-      <c r="C8">
-        <v>0.50133514404296797</v>
-      </c>
-      <c r="D8">
-        <v>1.7250130176544101</v>
-      </c>
-      <c r="E8">
-        <v>2.6360216140746999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>-1.0563949346542301</v>
-      </c>
-      <c r="C9">
-        <v>0.76382696628570501</v>
-      </c>
-      <c r="D9">
-        <v>1.5905055999755799</v>
-      </c>
-      <c r="E9">
-        <v>2.6506259441375701</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>0.27736204862594599</v>
-      </c>
-      <c r="C10">
-        <v>0.55775624513626099</v>
-      </c>
-      <c r="D10">
-        <v>1.3732042312621999</v>
-      </c>
-      <c r="E10">
-        <v>2.2170286178588801</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>-0.26222738623619002</v>
-      </c>
-      <c r="C11">
-        <v>1.06166136264801</v>
-      </c>
-      <c r="D11">
-        <v>1.2756724357604901</v>
-      </c>
-      <c r="E11">
-        <v>2.5947744846343901</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>-2.0087616443634002</v>
-      </c>
-      <c r="C12">
-        <v>0.68005710840225198</v>
-      </c>
-      <c r="D12">
-        <v>1.2625902891159</v>
-      </c>
-      <c r="E12">
-        <v>2.6184096336364702</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>-6.5937290191650302</v>
-      </c>
-      <c r="C13">
-        <v>0.51123619079589799</v>
-      </c>
-      <c r="D13">
-        <v>1.3422158956527701</v>
-      </c>
-      <c r="E13">
-        <v>2.8019282817840501</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E49F2D1-14B2-4EC2-9544-01485EF4F928}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>0.42047146000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>1.2615064</v>
-      </c>
-      <c r="C4">
-        <v>71.131397000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>-1.2937481</v>
-      </c>
-      <c r="C5">
-        <v>-78.024443000000005</v>
-      </c>
-      <c r="D5">
-        <v>85.607640000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6">
-        <v>0.18843132000000001</v>
-      </c>
-      <c r="C6">
-        <v>8.1101442000000006</v>
-      </c>
-      <c r="D6">
-        <v>-8.8726929999999999</v>
-      </c>
-      <c r="E6">
-        <v>1.1692260999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7">
-        <v>0.42047146000000002</v>
-      </c>
-      <c r="C7">
-        <v>1.2615064</v>
-      </c>
-      <c r="D7">
-        <v>-1.2937481</v>
-      </c>
-      <c r="E7">
-        <v>0.18843132000000001</v>
-      </c>
-      <c r="F7">
-        <v>0.42047146000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
-        <v>1.2615064</v>
-      </c>
-      <c r="C8">
-        <v>71.131397000000007</v>
-      </c>
-      <c r="D8">
-        <v>-78.024443000000005</v>
-      </c>
-      <c r="E8">
-        <v>8.1101442000000006</v>
-      </c>
-      <c r="F8">
-        <v>1.2615064</v>
-      </c>
-      <c r="G8">
-        <v>71.131397000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <v>-1.2937481</v>
-      </c>
-      <c r="C9">
-        <v>-78.024443000000005</v>
-      </c>
-      <c r="D9">
-        <v>85.607640000000004</v>
-      </c>
-      <c r="E9">
-        <v>-8.8726929999999999</v>
-      </c>
-      <c r="F9">
-        <v>-1.2937481</v>
-      </c>
-      <c r="G9">
-        <v>-78.024443000000005</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38332D03-B727-46AC-AFEF-80C1DCAC7D58}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>5.5318279999999997E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>7.43131E-3</v>
-      </c>
-      <c r="C4">
-        <v>1.65262E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>-8.4337700000000002E-3</v>
-      </c>
-      <c r="C5">
-        <v>-2.1088299999999999E-3</v>
-      </c>
-      <c r="D5">
-        <v>2.7433700000000002E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6">
-        <v>7.4016620000000005E-2</v>
-      </c>
-      <c r="C6">
-        <v>1.260929E-2</v>
-      </c>
-      <c r="D6">
-        <v>-1.51361E-2</v>
-      </c>
-      <c r="E6">
-        <v>0.11819185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7">
-        <v>5.5318279999999997E-2</v>
-      </c>
-      <c r="C7">
-        <v>7.43131E-3</v>
-      </c>
-      <c r="D7">
-        <v>-8.4337700000000002E-3</v>
-      </c>
-      <c r="E7">
-        <v>7.4016620000000005E-2</v>
-      </c>
-      <c r="F7">
-        <v>5.5318279999999997E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
-        <v>7.43131E-3</v>
-      </c>
-      <c r="C8">
-        <v>1.65262E-3</v>
-      </c>
-      <c r="D8">
-        <v>-2.1088299999999999E-3</v>
-      </c>
-      <c r="E8">
-        <v>1.260929E-2</v>
-      </c>
-      <c r="F8">
-        <v>7.43131E-3</v>
-      </c>
-      <c r="G8">
-        <v>1.65262E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <v>-8.4337700000000002E-3</v>
-      </c>
-      <c r="C9">
-        <v>-2.1088299999999999E-3</v>
-      </c>
-      <c r="D9">
-        <v>2.7433700000000002E-3</v>
-      </c>
-      <c r="E9">
-        <v>-1.51361E-2</v>
-      </c>
-      <c r="F9">
-        <v>-8.4337700000000002E-3</v>
-      </c>
-      <c r="G9">
-        <v>-2.1088299999999999E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C3AE16-EB21-4284-99CF-0CA9218C00BB}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>0.56969444999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>0.10252329</v>
-      </c>
-      <c r="C4">
-        <v>2.6091989999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>-0.10939767</v>
-      </c>
-      <c r="C5">
-        <v>-3.1290480000000002E-2</v>
-      </c>
-      <c r="D5">
-        <v>3.8674159999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6">
-        <v>0.27300596999999999</v>
-      </c>
-      <c r="C6">
-        <v>7.3005249999999994E-2</v>
-      </c>
-      <c r="D6">
-        <v>-8.7417289999999995E-2</v>
-      </c>
-      <c r="E6">
-        <v>0.24812039</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7">
-        <v>0.56969444999999996</v>
-      </c>
-      <c r="C7">
-        <v>0.10252329</v>
-      </c>
-      <c r="D7">
-        <v>-0.10939767</v>
-      </c>
-      <c r="E7">
-        <v>0.27300596999999999</v>
-      </c>
-      <c r="F7">
-        <v>0.56969444999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
-        <v>0.10252329</v>
-      </c>
-      <c r="C8">
-        <v>2.6091989999999999E-2</v>
-      </c>
-      <c r="D8">
-        <v>-3.1290480000000002E-2</v>
-      </c>
-      <c r="E8">
-        <v>7.3005249999999994E-2</v>
-      </c>
-      <c r="F8">
-        <v>0.10252329</v>
-      </c>
-      <c r="G8">
-        <v>2.6091989999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <v>-0.10939767</v>
-      </c>
-      <c r="C9">
-        <v>-3.1290480000000002E-2</v>
-      </c>
-      <c r="D9">
-        <v>3.8674159999999999E-2</v>
-      </c>
-      <c r="E9">
-        <v>-8.7417289999999995E-2</v>
-      </c>
-      <c r="F9">
-        <v>-0.10939767</v>
-      </c>
-      <c r="G9">
-        <v>-3.1290480000000002E-2</v>
+        <v>1.1756020000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2357,15 +2398,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6760BE32-F139-4EDF-B1ED-51D0BE4C1296}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -2384,8 +2425,11 @@
       <c r="G1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -2404,121 +2448,127 @@
       <c r="G2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3">
-        <v>9.241104E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>3.9047230000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4">
-        <v>1.6527719999999999E-2</v>
+        <v>4.3109699999999999E-3</v>
       </c>
       <c r="C4">
-        <v>4.5199000000000003E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>8.9881E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-1.8061589999999999E-2</v>
+        <v>-4.8614499999999998E-3</v>
       </c>
       <c r="C5">
-        <v>-5.6003600000000004E-3</v>
+        <v>-1.1485200000000001E-3</v>
       </c>
       <c r="D5">
-        <v>7.13351E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1.4912300000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6">
-        <v>5.5314269999999999E-2</v>
+        <v>7.2033680000000003E-2</v>
       </c>
       <c r="C6">
-        <v>1.441041E-2</v>
+        <v>1.0387850000000001E-2</v>
       </c>
       <c r="D6">
-        <v>-1.7332859999999999E-2</v>
+        <v>-1.241654E-2</v>
       </c>
       <c r="E6">
-        <v>5.7483449999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>0.15475742000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7">
-        <v>9.241104E-2</v>
+        <v>3.9047230000000002E-2</v>
       </c>
       <c r="C7">
-        <v>1.6527719999999999E-2</v>
+        <v>4.3109699999999999E-3</v>
       </c>
       <c r="D7">
-        <v>-1.8061589999999999E-2</v>
+        <v>-4.8614499999999998E-3</v>
       </c>
       <c r="E7">
-        <v>5.5314269999999999E-2</v>
+        <v>7.2033680000000003E-2</v>
       </c>
       <c r="F7">
-        <v>9.241104E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>3.9047230000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8">
-        <v>1.6527719999999999E-2</v>
+        <v>4.3109699999999999E-3</v>
       </c>
       <c r="C8">
-        <v>4.5199000000000003E-3</v>
+        <v>8.9881E-4</v>
       </c>
       <c r="D8">
-        <v>-5.6003600000000004E-3</v>
+        <v>-1.1485200000000001E-3</v>
       </c>
       <c r="E8">
-        <v>1.441041E-2</v>
+        <v>1.0387850000000001E-2</v>
       </c>
       <c r="F8">
-        <v>1.6527719999999999E-2</v>
+        <v>4.3109699999999999E-3</v>
       </c>
       <c r="G8">
-        <v>4.5199000000000003E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>8.9881E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-1.8061589999999999E-2</v>
+        <v>-4.8614499999999998E-3</v>
       </c>
       <c r="C9">
-        <v>-5.6003600000000004E-3</v>
+        <v>-1.1485200000000001E-3</v>
       </c>
       <c r="D9">
-        <v>7.13351E-3</v>
+        <v>1.4912300000000001E-3</v>
       </c>
       <c r="E9">
-        <v>-1.7332859999999999E-2</v>
+        <v>-1.241654E-2</v>
       </c>
       <c r="F9">
-        <v>-1.8061589999999999E-2</v>
+        <v>-4.8614499999999998E-3</v>
       </c>
       <c r="G9">
-        <v>-5.6003600000000004E-3</v>
+        <v>-1.1485200000000001E-3</v>
+      </c>
+      <c r="H9">
+        <v>1.4912300000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2528,15 +2578,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B91EEF-CDAB-4F7B-ABA3-4E6266E86A22}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -2555,8 +2605,11 @@
       <c r="G1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -2575,121 +2628,127 @@
       <c r="G2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3">
-        <v>0.70636441999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>0.43831226000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4">
-        <v>0.22945457999999999</v>
+        <v>6.1401810000000001E-2</v>
       </c>
       <c r="C4">
-        <v>8.760954E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1.478906E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-0.17408932999999999</v>
+        <v>-7.4411599999999994E-2</v>
       </c>
       <c r="C5">
-        <v>-7.1176409999999996E-2</v>
+        <v>-2.0922530000000002E-2</v>
       </c>
       <c r="D5">
-        <v>5.9392920000000002E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>3.0487429999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6">
-        <v>-5.9708219999999999E-2</v>
+        <v>0.40511542</v>
       </c>
       <c r="C6">
-        <v>2.6188499999999998E-3</v>
+        <v>8.3351170000000002E-2</v>
       </c>
       <c r="D6">
-        <v>-8.2103000000000002E-3</v>
+        <v>-0.11234065</v>
       </c>
       <c r="E6">
-        <v>8.3620609999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>0.55896829999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7">
-        <v>0.70636441999999999</v>
+        <v>0.43831226000000001</v>
       </c>
       <c r="C7">
-        <v>0.22945457999999999</v>
+        <v>6.1401810000000001E-2</v>
       </c>
       <c r="D7">
-        <v>-0.17408932999999999</v>
+        <v>-7.4411599999999994E-2</v>
       </c>
       <c r="E7">
-        <v>-5.9708219999999999E-2</v>
+        <v>0.40511542</v>
       </c>
       <c r="F7">
-        <v>0.70636441999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>0.43831226000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8">
-        <v>0.22945457999999999</v>
+        <v>6.1401810000000001E-2</v>
       </c>
       <c r="C8">
-        <v>8.760954E-2</v>
+        <v>1.478906E-2</v>
       </c>
       <c r="D8">
-        <v>-7.1176409999999996E-2</v>
+        <v>-2.0922530000000002E-2</v>
       </c>
       <c r="E8">
-        <v>2.6188499999999998E-3</v>
+        <v>8.3351170000000002E-2</v>
       </c>
       <c r="F8">
-        <v>0.22945457999999999</v>
+        <v>6.1401810000000001E-2</v>
       </c>
       <c r="G8">
-        <v>8.760954E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1.478906E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-0.17408932999999999</v>
+        <v>-7.4411599999999994E-2</v>
       </c>
       <c r="C9">
-        <v>-7.1176409999999996E-2</v>
+        <v>-2.0922530000000002E-2</v>
       </c>
       <c r="D9">
-        <v>5.9392920000000002E-2</v>
+        <v>3.0487429999999999E-2</v>
       </c>
       <c r="E9">
-        <v>-8.2103000000000002E-3</v>
+        <v>-0.11234065</v>
       </c>
       <c r="F9">
-        <v>-0.17408932999999999</v>
+        <v>-7.4411599999999994E-2</v>
       </c>
       <c r="G9">
-        <v>-7.1176409999999996E-2</v>
+        <v>-2.0922530000000002E-2</v>
+      </c>
+      <c r="H9">
+        <v>3.0487429999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2699,15 +2758,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6FA7F4-8E67-47E3-81E2-416898AAAC3B}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G9"/>
+      <selection sqref="A1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -2726,8 +2785,11 @@
       <c r="G1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -2746,121 +2808,127 @@
       <c r="G2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3">
-        <v>2.3806886</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>0.30559715999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4">
-        <v>2.2757955000000001</v>
+        <v>6.2411759999999997E-2</v>
       </c>
       <c r="C4">
-        <v>3.4321758999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>2.7844839999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-1.5834815</v>
+        <v>-5.9742820000000002E-2</v>
       </c>
       <c r="C5">
-        <v>-2.8071348</v>
+        <v>-3.2371080000000003E-2</v>
       </c>
       <c r="D5">
-        <v>2.3879427999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>3.8817049999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6">
-        <v>0.23198969999999999</v>
+        <v>0.29349468000000001</v>
       </c>
       <c r="C6">
-        <v>0.80907625000000005</v>
+        <v>9.6154439999999994E-2</v>
       </c>
       <c r="D6">
-        <v>-0.74656038999999996</v>
+        <v>-0.100565</v>
       </c>
       <c r="E6">
-        <v>0.45166137000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>0.56086842000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7">
-        <v>2.3806886</v>
+        <v>0.30559715999999998</v>
       </c>
       <c r="C7">
-        <v>2.2757955000000001</v>
+        <v>6.2411759999999997E-2</v>
       </c>
       <c r="D7">
-        <v>-1.5834815</v>
+        <v>-5.9742820000000002E-2</v>
       </c>
       <c r="E7">
-        <v>0.23198969999999999</v>
+        <v>0.29349468000000001</v>
       </c>
       <c r="F7">
-        <v>2.3806886</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>0.30559715999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8">
-        <v>2.2757955000000001</v>
+        <v>6.2411759999999997E-2</v>
       </c>
       <c r="C8">
-        <v>3.4321758999999998</v>
+        <v>2.7844839999999999E-2</v>
       </c>
       <c r="D8">
-        <v>-2.8071348</v>
+        <v>-3.2371080000000003E-2</v>
       </c>
       <c r="E8">
-        <v>0.80907625000000005</v>
+        <v>9.6154439999999994E-2</v>
       </c>
       <c r="F8">
-        <v>2.2757955000000001</v>
+        <v>6.2411759999999997E-2</v>
       </c>
       <c r="G8">
-        <v>3.4321758999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>2.7844839999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-1.5834815</v>
+        <v>-5.9742820000000002E-2</v>
       </c>
       <c r="C9">
-        <v>-2.8071348</v>
+        <v>-3.2371080000000003E-2</v>
       </c>
       <c r="D9">
-        <v>2.3879427999999998</v>
+        <v>3.8817049999999999E-2</v>
       </c>
       <c r="E9">
-        <v>-0.74656038999999996</v>
+        <v>-0.100565</v>
       </c>
       <c r="F9">
-        <v>-1.5834815</v>
+        <v>-5.9742820000000002E-2</v>
       </c>
       <c r="G9">
-        <v>-2.8071348</v>
+        <v>-3.2371080000000003E-2</v>
+      </c>
+      <c r="H9">
+        <v>3.8817049999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2873,7 +2941,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2929,7 +2997,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>0.57527521999999998</v>
+        <v>0.44132528999999998</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2937,10 +3005,10 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>9.4986760000000003E-2</v>
+        <v>5.383549E-2</v>
       </c>
       <c r="C4">
-        <v>2.1527379999999999E-2</v>
+        <v>8.4219199999999994E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2948,13 +3016,13 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>-0.1059372</v>
+        <v>-6.3206579999999998E-2</v>
       </c>
       <c r="C5">
-        <v>-2.8231800000000001E-2</v>
+        <v>-1.1113899999999999E-2</v>
       </c>
       <c r="D5">
-        <v>3.946761E-2</v>
+        <v>1.5332800000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2962,16 +3030,16 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>0.19848943999999999</v>
+        <v>0.32693750999999999</v>
       </c>
       <c r="C6">
-        <v>5.1533509999999998E-2</v>
+        <v>4.8476989999999998E-2</v>
       </c>
       <c r="D6">
-        <v>-6.736955E-2</v>
+        <v>-6.1565269999999998E-2</v>
       </c>
       <c r="E6">
-        <v>0.21335344000000001</v>
+        <v>0.32215264999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2979,19 +3047,19 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>0.57527521999999998</v>
+        <v>0.44132528999999998</v>
       </c>
       <c r="C7">
-        <v>9.4986760000000003E-2</v>
+        <v>5.383549E-2</v>
       </c>
       <c r="D7">
-        <v>-0.1059372</v>
+        <v>-6.3206579999999998E-2</v>
       </c>
       <c r="E7">
-        <v>0.19848943999999999</v>
+        <v>0.32693750999999999</v>
       </c>
       <c r="F7">
-        <v>0.57527521999999998</v>
+        <v>0.44132528999999998</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2999,22 +3067,22 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>9.4986760000000003E-2</v>
+        <v>5.383549E-2</v>
       </c>
       <c r="C8">
-        <v>2.1527379999999999E-2</v>
+        <v>8.4219199999999994E-3</v>
       </c>
       <c r="D8">
-        <v>-2.8231800000000001E-2</v>
+        <v>-1.1113899999999999E-2</v>
       </c>
       <c r="E8">
-        <v>5.1533509999999998E-2</v>
+        <v>4.8476989999999998E-2</v>
       </c>
       <c r="F8">
-        <v>9.4986760000000003E-2</v>
+        <v>5.383549E-2</v>
       </c>
       <c r="G8">
-        <v>2.1527379999999999E-2</v>
+        <v>8.4219199999999994E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3022,25 +3090,25 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>-0.1059372</v>
+        <v>-6.3206579999999998E-2</v>
       </c>
       <c r="C9">
-        <v>-2.8231800000000001E-2</v>
+        <v>-1.1113899999999999E-2</v>
       </c>
       <c r="D9">
-        <v>3.946761E-2</v>
+        <v>1.5332800000000001E-2</v>
       </c>
       <c r="E9">
-        <v>-6.736955E-2</v>
+        <v>-6.1565269999999998E-2</v>
       </c>
       <c r="F9">
-        <v>-0.1059372</v>
+        <v>-6.3206579999999998E-2</v>
       </c>
       <c r="G9">
-        <v>-2.8231800000000001E-2</v>
+        <v>-1.1113899999999999E-2</v>
       </c>
       <c r="H9">
-        <v>3.946761E-2</v>
+        <v>1.5332800000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Splines depend on implant (not costs/utilities yet)
</commit_message>
<xml_diff>
--- a/data/55-64_Female_first_revision.xlsx
+++ b/data/55-64_Female_first_revision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/KNIPS/code/KNIPS-Semi-Markov/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E234CD4E-6FE2-4C48-B089-81DE901C8A54}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FF8A4C3-2AA1-40FA-98FD-7BBE3015726F}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rcs_first_revision_mean" sheetId="1" r:id="rId1"/>
@@ -1427,7 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916FC4D9-7F7F-4ABB-88CF-874043B3D3E6}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1605,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8BE34F-251A-4B02-9EAF-7B6C81E08782}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1616,7 +1616,7 @@
     <col min="1" max="1" width="27.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>2.1021120548248202</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>2.7754933834075901</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>2.72922539710998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>2.7851717472076398</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>2.6451985836028999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>2.4115531444549498</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>2.6535215377807599</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>2.6937572956085201</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>2.5960001945495601</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>2.5343158245086599</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>2.5390820503234801</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1834,20 +1834,6 @@
         <v>1.27720034122467</v>
       </c>
       <c r="E13">
-        <v>2.2933709621429399</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16">
-        <v>-3.3356328010559002</v>
-      </c>
-      <c r="D16">
-        <v>0.423776924610137</v>
-      </c>
-      <c r="E16">
-        <v>1.27720034122467</v>
-      </c>
-      <c r="F16">
         <v>2.2933709621429399</v>
       </c>
     </row>

</xml_diff>